<commit_message>
permohonan + inv barang
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/permohonan_barang.xlsx
+++ b/public/files/template/inventory/permohonan_barang.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\public_html\epuskesmas_prog\dev\public\files\template\inventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projek\newepuskesmas\public\files\template\inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>No</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Inventory - Daftar Permohonan Barang</t>
+  </si>
+  <si>
+    <t>Total Harga (Rp.)</t>
+  </si>
+  <si>
+    <t>[a.totalharga]</t>
   </si>
 </sst>
 </file>
@@ -141,7 +147,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -157,13 +163,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:G7" totalsRowShown="0">
-  <autoFilter ref="B6:G7"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:H7" totalsRowShown="0">
+  <autoFilter ref="B6:H7"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="No"/>
     <tableColumn id="2" name="Tanggal Permohonan" dataDxfId="0"/>
     <tableColumn id="3" name="Puskesmas Ruangan"/>
     <tableColumn id="4" name="Jumlah Barang"/>
+    <tableColumn id="7" name="Total Harga (Rp.)"/>
     <tableColumn id="5" name="Keterangan"/>
     <tableColumn id="6" name="Status"/>
   </tableColumns>
@@ -434,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,19 +453,20 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -466,7 +474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -480,13 +488,16 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -500,9 +511,12 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>